<commit_message>
Inicio dos experimentos. Planilha atualizada
</commit_message>
<xml_diff>
--- a/_experimentos/Análise01/Experimentos.xlsx
+++ b/_experimentos/Análise01/Experimentos.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Base de dados" sheetId="1" r:id="rId1"/>
-    <sheet name="Experimentos 01" sheetId="2" r:id="rId2"/>
+    <sheet name="Experimentos" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Base de dados</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>(CODE)</t>
+  </si>
+  <si>
+    <t>Experimentos</t>
+  </si>
+  <si>
+    <t>DEFAULT (with parallel)</t>
   </si>
 </sst>
 </file>
@@ -138,7 +144,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -160,6 +166,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -445,7 +454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -513,23 +522,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D4" sqref="D4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="B1" s="7" t="s">
         <v>19</v>
       </c>
@@ -544,7 +558,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
       <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
@@ -565,7 +580,10 @@
       </c>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
       <c r="B3" t="s">
         <v>20</v>
       </c>
@@ -588,11 +606,32 @@
         <v>0.1531279178338</v>
       </c>
     </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
experimentos com cluster, planilha atualizada
</commit_message>
<xml_diff>
--- a/_experimentos/Análise01/Experimentos.xlsx
+++ b/_experimentos/Análise01/Experimentos.xlsx
@@ -525,7 +525,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:F4"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,6 +625,12 @@
       <c r="F4">
         <v>20</v>
       </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>0.17740429505135399</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Fim dos experimentos - update tabela resultados
</commit_message>
<xml_diff>
--- a/_experimentos/Análise01/Experimentos.xlsx
+++ b/_experimentos/Análise01/Experimentos.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="100">
   <si>
     <t>Base de dados</t>
   </si>
@@ -316,6 +316,12 @@
   </si>
   <si>
     <t>Redução (%)</t>
+  </si>
+  <si>
+    <t>(CODE with parallel - both)</t>
+  </si>
+  <si>
+    <t>Tolerance</t>
   </si>
 </sst>
 </file>
@@ -750,26 +756,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="48.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>22</v>
       </c>
@@ -783,12 +790,13 @@
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="5" t="s">
         <v>11</v>
@@ -803,17 +811,20 @@
         <v>16</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -829,20 +840,20 @@
       <c r="E3">
         <v>100</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>20</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>92</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.1531279178338</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -858,20 +869,20 @@
       <c r="E4">
         <v>100</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>20</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>100</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>25</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.17740429505135399</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -887,44 +898,79 @@
       <c r="E5">
         <v>100</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>20</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>100</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.134920634920635</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6">
         <v>200</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>20</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>86</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.13538748832866501</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>200</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>77</v>
+      </c>
+      <c r="J7">
+        <v>0.135854341736695</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="J1:J2"/>
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>